<commit_message>
feat(delta): Load missing translations
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/Bhasha_Daan_All_Content_August_5.xlsx
+++ b/utils/localization/resources/backup/Bhasha_Daan_All_Content_August_5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localization/resources/backup/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5E91805-671D-9045-8498-CDAD01AAA0D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C6683A-7CC0-4C40-A260-1C43A2DCE38E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17003,32 +17003,6 @@
     <t>ಚಿತ್ರಗಳ ಲೇಬಲ್‌ಗಳು</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>Translated &lt;contribution-count&gt; &lt;language&gt; &lt;s&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF4A86E8"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>sentence(s)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t>&lt;/s&gt;</t>
-    </r>
-  </si>
-  <si>
     <t>&lt;contribution-count&gt; &lt;language&gt; &lt;s&gt;वाक्य&lt;/s&gt; अनुवादित</t>
   </si>
   <si>
@@ -17114,10 +17088,6 @@
   </si>
   <si>
     <t>&lt;validation-count&gt; &lt;language&gt; &lt;s&gt; ವಾಕ್ಯ (ಗಳು) &lt;/ s&gt; ಮೌಲ್ಯೀಕರಿಸಲ್ಪಟ್ಟಿವೆ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You have changed the contribution language from &lt;old language&gt; to &lt;new language&gt;, we will be redirecting you to homepage to start participating again.
-</t>
   </si>
   <si>
     <t>आपने  योगदान की भाषा को &lt;old language&gt; से &lt;new language&gt;, में बदल दिया है, फिर से भाग लेने के लिए आपको होमपेज पर रिडायरेक्ट किया जाएगा।</t>
@@ -17400,6 +17370,30 @@
   </si>
   <si>
     <t>ଆପଣ &lt;v&gt; ରେକର୍ଡିଂ ଯୋଗଦାନ କରି ଏକ &lt;u&gt; ଭାଷା ସମର୍ଥକ ବ୍ୟାଜ୍ ଅର୍ଜନ କରିଛନ୍ତି</t>
+  </si>
+  <si>
+    <t>You have changed the contribution language from &lt;old language&gt; to &lt;new language&gt;, we will be redirecting you to homepage to start participating again.</t>
+  </si>
+  <si>
+    <r>
+      <t>Translated &lt;contribution-count&gt; &lt;language&gt; &lt;s&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF4A86E8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>sentence(s)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>&lt;/s&gt;</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -17956,9 +17950,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A358" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E380" sqref="E380"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A437" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A466" sqref="A466"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -39894,13 +39888,13 @@
         <v>4789</v>
       </c>
       <c r="D428" s="8" t="s">
-        <v>5310</v>
+        <v>5308</v>
       </c>
       <c r="E428" s="6" t="s">
         <v>4790</v>
       </c>
       <c r="F428" s="4" t="s">
-        <v>5318</v>
+        <v>5316</v>
       </c>
       <c r="G428" s="9" t="s">
         <v>4791</v>
@@ -39918,7 +39912,7 @@
         <v>4795</v>
       </c>
       <c r="L428" s="9" t="s">
-        <v>5336</v>
+        <v>5334</v>
       </c>
       <c r="M428" s="2"/>
       <c r="N428" s="2"/>
@@ -39943,19 +39937,19 @@
         <v>4797</v>
       </c>
       <c r="C429" s="4" t="s">
-        <v>5307</v>
+        <v>5305</v>
       </c>
       <c r="D429" s="8" t="s">
-        <v>5311</v>
+        <v>5309</v>
       </c>
       <c r="E429" s="6" t="s">
         <v>4798</v>
       </c>
       <c r="F429" s="4" t="s">
-        <v>5319</v>
+        <v>5317</v>
       </c>
       <c r="G429" s="9" t="s">
-        <v>5339</v>
+        <v>5337</v>
       </c>
       <c r="H429" s="4" t="s">
         <v>4799</v>
@@ -39970,7 +39964,7 @@
         <v>4802</v>
       </c>
       <c r="L429" s="9" t="s">
-        <v>5337</v>
+        <v>5335</v>
       </c>
       <c r="M429" s="2"/>
       <c r="N429" s="2"/>
@@ -40102,13 +40096,13 @@
         <v>4829</v>
       </c>
       <c r="D432" s="8" t="s">
-        <v>5312</v>
+        <v>5310</v>
       </c>
       <c r="E432" s="6" t="s">
         <v>4830</v>
       </c>
       <c r="F432" s="4" t="s">
-        <v>5320</v>
+        <v>5318</v>
       </c>
       <c r="G432" s="9" t="s">
         <v>4831</v>
@@ -40154,13 +40148,13 @@
         <v>4839</v>
       </c>
       <c r="D433" s="8" t="s">
-        <v>5313</v>
+        <v>5311</v>
       </c>
       <c r="E433" s="6" t="s">
         <v>4840</v>
       </c>
       <c r="F433" s="4" t="s">
-        <v>5321</v>
+        <v>5319</v>
       </c>
       <c r="G433" s="9" t="s">
         <v>4841</v>
@@ -40258,13 +40252,13 @@
         <v>4860</v>
       </c>
       <c r="D435" s="8" t="s">
-        <v>5314</v>
+        <v>5312</v>
       </c>
       <c r="E435" s="6" t="s">
         <v>4861</v>
       </c>
       <c r="F435" s="4" t="s">
-        <v>5322</v>
+        <v>5320</v>
       </c>
       <c r="G435" s="9" t="s">
         <v>4862</v>
@@ -40310,13 +40304,13 @@
         <v>4870</v>
       </c>
       <c r="D436" s="8" t="s">
-        <v>5315</v>
+        <v>5313</v>
       </c>
       <c r="E436" s="6" t="s">
         <v>4871</v>
       </c>
       <c r="F436" s="4" t="s">
-        <v>5323</v>
+        <v>5321</v>
       </c>
       <c r="G436" s="9" t="s">
         <v>4872</v>
@@ -40362,13 +40356,13 @@
         <v>4880</v>
       </c>
       <c r="D437" s="8" t="s">
-        <v>5316</v>
+        <v>5314</v>
       </c>
       <c r="E437" s="6" t="s">
         <v>4881</v>
       </c>
       <c r="F437" s="4" t="s">
-        <v>5324</v>
+        <v>5322</v>
       </c>
       <c r="G437" s="9" t="s">
         <v>4882</v>
@@ -40992,7 +40986,7 @@
         <v>5016</v>
       </c>
       <c r="F449" s="4" t="s">
-        <v>5325</v>
+        <v>5323</v>
       </c>
       <c r="G449" s="9" t="s">
         <v>5017</v>
@@ -41004,7 +40998,7 @@
         <v>5019</v>
       </c>
       <c r="J449" s="4" t="s">
-        <v>5331</v>
+        <v>5329</v>
       </c>
       <c r="K449" s="6" t="s">
         <v>5020</v>
@@ -41035,7 +41029,7 @@
         <v>5023</v>
       </c>
       <c r="C450" s="4" t="s">
-        <v>5308</v>
+        <v>5306</v>
       </c>
       <c r="D450" s="8" t="s">
         <v>5024</v>
@@ -41044,7 +41038,7 @@
         <v>5025</v>
       </c>
       <c r="F450" s="4" t="s">
-        <v>5326</v>
+        <v>5324</v>
       </c>
       <c r="G450" s="9" t="s">
         <v>5026</v>
@@ -41056,7 +41050,7 @@
         <v>5028</v>
       </c>
       <c r="J450" s="4" t="s">
-        <v>5332</v>
+        <v>5330</v>
       </c>
       <c r="K450" s="6" t="s">
         <v>5029</v>
@@ -41090,13 +41084,13 @@
         <v>5033</v>
       </c>
       <c r="D451" s="8" t="s">
-        <v>5317</v>
+        <v>5315</v>
       </c>
       <c r="E451" s="6" t="s">
         <v>5034</v>
       </c>
       <c r="F451" s="4" t="s">
-        <v>5327</v>
+        <v>5325</v>
       </c>
       <c r="G451" s="9" t="s">
         <v>5035</v>
@@ -41108,7 +41102,7 @@
         <v>5037</v>
       </c>
       <c r="J451" s="4" t="s">
-        <v>5333</v>
+        <v>5331</v>
       </c>
       <c r="K451" s="6" t="s">
         <v>5038</v>
@@ -41148,7 +41142,7 @@
         <v>5044</v>
       </c>
       <c r="F452" s="4" t="s">
-        <v>5328</v>
+        <v>5326</v>
       </c>
       <c r="G452" s="9" t="s">
         <v>5045</v>
@@ -41160,7 +41154,7 @@
         <v>5047</v>
       </c>
       <c r="J452" s="4" t="s">
-        <v>5334</v>
+        <v>5332</v>
       </c>
       <c r="K452" s="6" t="s">
         <v>5048</v>
@@ -41188,10 +41182,10 @@
         <v>5050</v>
       </c>
       <c r="B453" s="4" t="s">
-        <v>5306</v>
+        <v>5304</v>
       </c>
       <c r="C453" s="4" t="s">
-        <v>5309</v>
+        <v>5307</v>
       </c>
       <c r="D453" s="8" t="s">
         <v>5050</v>
@@ -41200,7 +41194,7 @@
         <v>5051</v>
       </c>
       <c r="F453" s="4" t="s">
-        <v>5329</v>
+        <v>5327</v>
       </c>
       <c r="G453" s="9" t="s">
         <v>5052</v>
@@ -41209,16 +41203,16 @@
         <v>5053</v>
       </c>
       <c r="I453" s="6" t="s">
-        <v>5330</v>
+        <v>5328</v>
       </c>
       <c r="J453" s="4" t="s">
-        <v>5335</v>
+        <v>5333</v>
       </c>
       <c r="K453" s="6" t="s">
-        <v>5340</v>
+        <v>5338</v>
       </c>
       <c r="L453" s="9" t="s">
-        <v>5338</v>
+        <v>5336</v>
       </c>
       <c r="M453" s="2"/>
       <c r="N453" s="2"/>
@@ -42139,38 +42133,38 @@
     </row>
     <row r="472" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A472" s="43" t="s">
+        <v>5340</v>
+      </c>
+      <c r="B472" s="44" t="s">
         <v>5236</v>
       </c>
-      <c r="B472" s="44" t="s">
+      <c r="C472" s="44" t="s">
         <v>5237</v>
-      </c>
-      <c r="C472" s="44" t="s">
-        <v>5238</v>
       </c>
       <c r="D472" s="35"/>
       <c r="E472" s="34" t="s">
+        <v>5238</v>
+      </c>
+      <c r="F472" s="34" t="s">
         <v>5239</v>
       </c>
-      <c r="F472" s="34" t="s">
+      <c r="G472" s="45" t="s">
         <v>5240</v>
       </c>
-      <c r="G472" s="45" t="s">
+      <c r="H472" s="34" t="s">
         <v>5241</v>
       </c>
-      <c r="H472" s="34" t="s">
+      <c r="I472" s="39" t="s">
         <v>5242</v>
       </c>
-      <c r="I472" s="39" t="s">
+      <c r="J472" s="34" t="s">
         <v>5243</v>
       </c>
-      <c r="J472" s="34" t="s">
+      <c r="K472" s="34" t="s">
         <v>5244</v>
       </c>
-      <c r="K472" s="34" t="s">
+      <c r="L472" s="42" t="s">
         <v>5245</v>
-      </c>
-      <c r="L472" s="42" t="s">
-        <v>5246</v>
       </c>
       <c r="M472" s="2"/>
       <c r="N472" s="2"/>
@@ -42189,38 +42183,38 @@
     </row>
     <row r="473" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A473" s="43" t="s">
+        <v>5246</v>
+      </c>
+      <c r="B473" s="44" t="s">
         <v>5247</v>
       </c>
-      <c r="B473" s="44" t="s">
+      <c r="C473" s="44" t="s">
         <v>5248</v>
-      </c>
-      <c r="C473" s="44" t="s">
-        <v>5249</v>
       </c>
       <c r="D473" s="35"/>
       <c r="E473" s="34" t="s">
+        <v>5249</v>
+      </c>
+      <c r="F473" s="34" t="s">
         <v>5250</v>
       </c>
-      <c r="F473" s="34" t="s">
+      <c r="G473" s="45" t="s">
         <v>5251</v>
       </c>
-      <c r="G473" s="45" t="s">
+      <c r="H473" s="34" t="s">
         <v>5252</v>
       </c>
-      <c r="H473" s="34" t="s">
+      <c r="I473" s="39" t="s">
         <v>5253</v>
       </c>
-      <c r="I473" s="39" t="s">
+      <c r="J473" s="34" t="s">
         <v>5254</v>
       </c>
-      <c r="J473" s="34" t="s">
+      <c r="K473" s="34" t="s">
         <v>5255</v>
       </c>
-      <c r="K473" s="34" t="s">
+      <c r="L473" s="42" t="s">
         <v>5256</v>
-      </c>
-      <c r="L473" s="42" t="s">
-        <v>5257</v>
       </c>
       <c r="M473" s="2"/>
       <c r="N473" s="2"/>
@@ -42239,38 +42233,38 @@
     </row>
     <row r="474" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A474" s="46" t="s">
+        <v>5339</v>
+      </c>
+      <c r="B474" s="47" t="s">
+        <v>5257</v>
+      </c>
+      <c r="C474" s="47" t="s">
         <v>5258</v>
-      </c>
-      <c r="B474" s="47" t="s">
-        <v>5259</v>
-      </c>
-      <c r="C474" s="47" t="s">
-        <v>5260</v>
       </c>
       <c r="D474" s="48"/>
       <c r="E474" s="47" t="s">
+        <v>5259</v>
+      </c>
+      <c r="F474" s="47" t="s">
+        <v>5260</v>
+      </c>
+      <c r="G474" s="49" t="s">
         <v>5261</v>
       </c>
-      <c r="F474" s="47" t="s">
+      <c r="H474" s="47" t="s">
         <v>5262</v>
       </c>
-      <c r="G474" s="49" t="s">
+      <c r="I474" s="47" t="s">
         <v>5263</v>
       </c>
-      <c r="H474" s="47" t="s">
+      <c r="J474" s="47" t="s">
         <v>5264</v>
       </c>
-      <c r="I474" s="47" t="s">
+      <c r="K474" s="47" t="s">
         <v>5265</v>
       </c>
-      <c r="J474" s="47" t="s">
+      <c r="L474" s="47" t="s">
         <v>5266</v>
-      </c>
-      <c r="K474" s="47" t="s">
-        <v>5267</v>
-      </c>
-      <c r="L474" s="47" t="s">
-        <v>5268</v>
       </c>
       <c r="M474" s="2"/>
       <c r="N474" s="2"/>
@@ -42289,38 +42283,38 @@
     </row>
     <row r="475" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A475" s="43" t="s">
+        <v>5267</v>
+      </c>
+      <c r="B475" s="47" t="s">
+        <v>5268</v>
+      </c>
+      <c r="C475" s="50" t="s">
         <v>5269</v>
-      </c>
-      <c r="B475" s="47" t="s">
-        <v>5270</v>
-      </c>
-      <c r="C475" s="50" t="s">
-        <v>5271</v>
       </c>
       <c r="D475" s="48"/>
       <c r="E475" s="47" t="s">
+        <v>5270</v>
+      </c>
+      <c r="F475" s="47" t="s">
+        <v>5271</v>
+      </c>
+      <c r="G475" s="51" t="s">
         <v>5272</v>
       </c>
-      <c r="F475" s="47" t="s">
+      <c r="H475" s="47" t="s">
         <v>5273</v>
       </c>
-      <c r="G475" s="51" t="s">
+      <c r="I475" s="47" t="s">
         <v>5274</v>
       </c>
-      <c r="H475" s="47" t="s">
+      <c r="J475" s="47" t="s">
         <v>5275</v>
       </c>
-      <c r="I475" s="47" t="s">
+      <c r="K475" s="47" t="s">
         <v>5276</v>
       </c>
-      <c r="J475" s="47" t="s">
+      <c r="L475" s="47" t="s">
         <v>5277</v>
-      </c>
-      <c r="K475" s="47" t="s">
-        <v>5278</v>
-      </c>
-      <c r="L475" s="47" t="s">
-        <v>5279</v>
       </c>
       <c r="M475" s="2"/>
       <c r="N475" s="2"/>
@@ -42339,38 +42333,38 @@
     </row>
     <row r="476" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A476" s="43" t="s">
+        <v>5278</v>
+      </c>
+      <c r="B476" s="47" t="s">
+        <v>5279</v>
+      </c>
+      <c r="C476" s="50" t="s">
         <v>5280</v>
-      </c>
-      <c r="B476" s="47" t="s">
-        <v>5281</v>
-      </c>
-      <c r="C476" s="50" t="s">
-        <v>5282</v>
       </c>
       <c r="D476" s="48"/>
       <c r="E476" s="47" t="s">
+        <v>5281</v>
+      </c>
+      <c r="F476" s="47" t="s">
+        <v>5282</v>
+      </c>
+      <c r="G476" s="52" t="s">
         <v>5283</v>
       </c>
-      <c r="F476" s="47" t="s">
+      <c r="H476" s="47" t="s">
         <v>5284</v>
       </c>
-      <c r="G476" s="52" t="s">
+      <c r="I476" s="47" t="s">
         <v>5285</v>
       </c>
-      <c r="H476" s="47" t="s">
+      <c r="J476" s="47" t="s">
         <v>5286</v>
       </c>
-      <c r="I476" s="47" t="s">
+      <c r="K476" s="47" t="s">
         <v>5287</v>
       </c>
-      <c r="J476" s="47" t="s">
+      <c r="L476" s="47" t="s">
         <v>5288</v>
-      </c>
-      <c r="K476" s="47" t="s">
-        <v>5289</v>
-      </c>
-      <c r="L476" s="47" t="s">
-        <v>5290</v>
       </c>
       <c r="M476" s="2"/>
       <c r="N476" s="2"/>
@@ -42399,7 +42393,7 @@
       </c>
       <c r="D477" s="48"/>
       <c r="E477" s="47" t="s">
-        <v>5291</v>
+        <v>5289</v>
       </c>
       <c r="F477" s="47" t="s">
         <v>4240</v>
@@ -42411,13 +42405,13 @@
         <v>4242</v>
       </c>
       <c r="I477" s="47" t="s">
+        <v>5290</v>
+      </c>
+      <c r="J477" s="47" t="s">
+        <v>5291</v>
+      </c>
+      <c r="K477" s="47" t="s">
         <v>5292</v>
-      </c>
-      <c r="J477" s="47" t="s">
-        <v>5293</v>
-      </c>
-      <c r="K477" s="47" t="s">
-        <v>5294</v>
       </c>
       <c r="L477" s="47" t="s">
         <v>4246</v>
@@ -42439,38 +42433,38 @@
     </row>
     <row r="478" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A478" s="53" t="s">
-        <v>5305</v>
+        <v>5303</v>
       </c>
       <c r="B478" s="4" t="s">
-        <v>5295</v>
+        <v>5293</v>
       </c>
       <c r="C478" s="4" t="s">
-        <v>5296</v>
+        <v>5294</v>
       </c>
       <c r="D478" s="54"/>
       <c r="E478" s="4" t="s">
+        <v>5295</v>
+      </c>
+      <c r="F478" s="4" t="s">
+        <v>5296</v>
+      </c>
+      <c r="G478" s="9" t="s">
         <v>5297</v>
       </c>
-      <c r="F478" s="4" t="s">
+      <c r="H478" s="4" t="s">
         <v>5298</v>
       </c>
-      <c r="G478" s="9" t="s">
+      <c r="I478" s="9" t="s">
         <v>5299</v>
       </c>
-      <c r="H478" s="4" t="s">
+      <c r="J478" s="4" t="s">
         <v>5300</v>
       </c>
-      <c r="I478" s="9" t="s">
+      <c r="K478" s="4" t="s">
         <v>5301</v>
       </c>
-      <c r="J478" s="4" t="s">
+      <c r="L478" s="9" t="s">
         <v>5302</v>
-      </c>
-      <c r="K478" s="4" t="s">
-        <v>5303</v>
-      </c>
-      <c r="L478" s="9" t="s">
-        <v>5304</v>
       </c>
       <c r="M478" s="55"/>
       <c r="N478" s="55"/>

</xml_diff>